<commit_message>
Updated dimensions documentation for rescaling
</commit_message>
<xml_diff>
--- a/AOSMapmaker/docs/dimensions.xlsx
+++ b/AOSMapmaker/docs/dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhipsher\git\localAOSMapMaker\AOSMapmaker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ADD00E-E083-4423-AD2E-AA3DDBE2C2FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC8428-8F79-475D-BEF7-58E5AEF514FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="4890" windowWidth="28800" windowHeight="15435" xr2:uid="{40905910-5CB8-4363-AAC9-7B82BA24352D}"/>
   </bookViews>
@@ -1468,7 +1468,7 @@
   <dimension ref="B4:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,12 +1711,12 @@
         <v>6</v>
       </c>
       <c r="D22" s="9">
-        <f>280*4</f>
-        <v>1120</v>
+        <f>280*4.6</f>
+        <v>1288</v>
       </c>
       <c r="E22" s="10">
         <f>ROUND(D22,0)</f>
-        <v>1120</v>
+        <v>1288</v>
       </c>
       <c r="F22" s="4">
         <f>(E22-D22)/D22</f>
@@ -1732,15 +1732,15 @@
       </c>
       <c r="D23">
         <f>D22*D17</f>
-        <v>865.45454545454538</v>
+        <v>995.27272727272725</v>
       </c>
       <c r="E23" s="11">
         <f>ROUND(D23,0)</f>
-        <v>865</v>
+        <v>995</v>
       </c>
       <c r="F23" s="4">
         <f>(E23-D23)/D23</f>
-        <v>-5.2521008403352994E-4</v>
+        <v>-2.7402265253925582E-4</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1755,19 +1755,19 @@
       </c>
       <c r="D25" s="18">
         <f>D22*D16+5</f>
-        <v>145.30064423765211</v>
+        <v>166.34574087329995</v>
       </c>
       <c r="E25" s="14">
         <f>ROUND(D25,0)</f>
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="F25" s="4">
         <f>(E25-D25)/D25</f>
-        <v>-2.0691184077640946E-3</v>
+        <v>-2.0784474040924485E-3</v>
       </c>
       <c r="G25" s="8" t="b">
         <f>ISEVEN(E25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>22</v>
@@ -1782,15 +1782,15 @@
       </c>
       <c r="D26" s="16">
         <f>D25*D18</f>
-        <v>167.77873212806898</v>
+        <v>192.07951654349489</v>
       </c>
       <c r="E26" s="16">
         <f>ROUND(D26,0)</f>
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F26" s="4">
         <f>(E26-D26)/D26</f>
-        <v>1.3188076290987865E-3</v>
+        <v>-4.1397721592496828E-4</v>
       </c>
       <c r="G26" s="8" t="b">
         <f>ISEVEN(E26)</f>
@@ -1809,19 +1809,19 @@
       </c>
       <c r="D27" s="14">
         <f>D25/2</f>
-        <v>72.650322118826054</v>
+        <v>83.172870436649973</v>
       </c>
       <c r="E27" s="15">
         <f>ROUND(D27,0)</f>
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F27" s="4">
         <f>(E27-D27)/D27</f>
-        <v>4.8131635342513251E-3</v>
+        <v>-2.0784474040924485E-3</v>
       </c>
       <c r="G27" s="8" t="b">
         <f>F27&lt;0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>29</v>
@@ -1836,19 +1836,19 @@
       </c>
       <c r="D28" s="12">
         <f>D25*D19</f>
-        <v>125.83404909605173</v>
+        <v>144.05963740762118</v>
       </c>
       <c r="E28" s="13">
         <f>ROUND(D28,0)</f>
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="F28" s="4">
         <f>(E28-D28)/D28</f>
-        <v>1.3188076290988431E-3</v>
+        <v>-4.1397721592506689E-4</v>
       </c>
       <c r="G28" s="8" t="b">
         <f>F28&lt;0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>23</v>
@@ -1863,19 +1863,19 @@
       </c>
       <c r="D29" s="16">
         <f>D26/2</f>
-        <v>83.88936606403449</v>
+        <v>96.039758271747445</v>
       </c>
       <c r="E29" s="17">
         <f>ROUND(D29,0)</f>
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F29" s="4">
         <f>(E29-D29)/D29</f>
-        <v>1.3188076290987865E-3</v>
+        <v>-4.1397721592496828E-4</v>
       </c>
       <c r="G29" s="8" t="b">
         <f>F29&lt;0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>39</v>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="D32">
         <f>D22/D25</f>
-        <v>7.7081557750572705</v>
+        <v>7.7429093960453548</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="3"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="D33">
         <f>D32</f>
-        <v>7.7081557750572705</v>
+        <v>7.7429093960453548</v>
       </c>
       <c r="E33" s="11">
         <f>FLOOR(D33,1)</f>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="F33" s="3">
         <f>(E33-D33)/D33</f>
-        <v>-9.1870973514674326E-2</v>
+        <v>-9.594706047119593E-2</v>
       </c>
       <c r="G33" s="8" t="b">
         <f>F33&lt;0</f>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="D34">
         <f>D33-0.5</f>
-        <v>7.2081557750572705</v>
+        <v>7.2429093960453548</v>
       </c>
       <c r="E34" s="11">
         <f>FLOOR(D34,1)</f>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="F34" s="3">
         <f>(E34-D34)/D34</f>
-        <v>-2.8877813070794327E-2</v>
+        <v>-3.35375444815013E-2</v>
       </c>
       <c r="G34" s="8" t="b">
         <f>F35&lt;0</f>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D35">
         <f>(D23-D26)/D28+1</f>
-        <v>6.5444120119978502</v>
+        <v>6.5754215766666997</v>
       </c>
       <c r="E35" s="11">
         <f>FLOOR(D35,1)</f>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="F35" s="3">
         <f>(E35-D35)/D35</f>
-        <v>-8.3187307125495963E-2</v>
+        <v>-8.7510978567308842E-2</v>
       </c>
       <c r="G35" s="8" t="b">
         <f>F35&lt;0</f>

</xml_diff>